<commit_message>
Commit RAP test case
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/MedicaRAP/3.3.0.0/accreditamento-checklist_V8.2.6.1.xlsx
+++ b/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/MedicaRAP/3.3.0.0/accreditamento-checklist_V8.2.6.1.xlsx
@@ -289,13 +289,13 @@
 Il Documento CDA2 Anatomia Patologica dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-11-21T14:48:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f17a52cc1f41dbaab06ea7aa380099ee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.2d9d1e1cb993a5ee9fdb693d95281b2e7a9a1782cd4943921fb6e364c984ef82.6f581e8737^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-12-01T11:03:03Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4cc289b3fb2ae7ee41d6e769ba9dfcf9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.ab52f709d42185722cf5bc88f736a97566a8cce97abad2fec8d91d5b928ef3ce.04291dd230^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -312,13 +312,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2025-11-21T14:52:21Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8fbe83e9283cb1064e36321294f2e904</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.ea2cb81792fff9badc3ae9cd39d33e4d1587752d36115bbdeba237d798931a22.5bbc49c8fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-12-01T11:08:56Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28cb5f4b6dcef3c48f737cb1e22917c3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.eafd82037364042d6cf61cf7ffe7e9092479d2db5649a6ed64e6fd145088d94d.4f70732b99^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAP_CT3</t>
@@ -729,13 +729,13 @@
 Il Documento CDA2 Anatomia Patologica dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-11-21T15:03:27Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7b29a3e8b044129c608d3f8f06e28a67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.d0997b2872be3beb3013bfecd5780c97847390739ce1fe6b584b9d9ec2e67d20.47d776b6d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-12-01T11:14:34Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c60caa2392ca927d9af21c6be6693619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.0ee933436c32eb3a041f2b388addeb1b62dfd53a9b4263585afb1f1a08fb3100.3b3424d27e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAP_CT25_KO</t>
@@ -1531,7 +1531,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.82"/>
@@ -1618,7 +1618,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.18"/>
@@ -2692,14 +2692,14 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="S10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
@@ -2998,7 +2998,7 @@
         <v>49</v>
       </c>
       <c r="F10" s="31" t="n">
-        <v>45982</v>
+        <v>45992</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>50</v>
@@ -3045,7 +3045,7 @@
         <v>56</v>
       </c>
       <c r="F11" s="31" t="n">
-        <v>45982</v>
+        <v>45992</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>57</v>
@@ -3878,7 +3878,7 @@
         <v>135</v>
       </c>
       <c r="F26" s="31" t="n">
-        <v>45982</v>
+        <v>45992</v>
       </c>
       <c r="G26" s="31" t="s">
         <v>136</v>
@@ -8068,7 +8068,7 @@
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -8134,7 +8134,7 @@
       <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
@@ -9282,7 +9282,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.17"/>

</xml_diff>

<commit_message>
Commit Anatomia Patoligica - aggiornamento check-list
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/MedicaRAP/3.3.0.0/accreditamento-checklist_V8.2.6.1.xlsx
+++ b/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/MedicaRAP/3.3.0.0/accreditamento-checklist_V8.2.6.1.xlsx
@@ -1550,11 +1550,11 @@
   </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.82"/>
@@ -1637,11 +1637,11 @@
   </sheetPr>
   <dimension ref="A1:B996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.18"/>
@@ -2714,15 +2714,15 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
@@ -3188,7 +3188,7 @@
         <v>62</v>
       </c>
       <c r="R13" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S13" s="38" t="s">
         <v>70</v>
@@ -3249,7 +3249,7 @@
         <v>62</v>
       </c>
       <c r="R14" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S14" s="38" t="s">
         <v>70</v>
@@ -3302,7 +3302,7 @@
         <v>62</v>
       </c>
       <c r="R15" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S15" s="38" t="s">
         <v>80</v>
@@ -3363,7 +3363,7 @@
         <v>62</v>
       </c>
       <c r="R16" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S16" s="39" t="s">
         <v>87</v>
@@ -3424,7 +3424,7 @@
         <v>62</v>
       </c>
       <c r="R17" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S17" s="39" t="s">
         <v>87</v>
@@ -3485,7 +3485,7 @@
         <v>62</v>
       </c>
       <c r="R18" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S18" s="39" t="s">
         <v>87</v>
@@ -3546,7 +3546,7 @@
         <v>62</v>
       </c>
       <c r="R19" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S19" s="39" t="s">
         <v>87</v>
@@ -3607,7 +3607,7 @@
         <v>62</v>
       </c>
       <c r="R20" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S20" s="39" t="s">
         <v>87</v>
@@ -3668,7 +3668,7 @@
         <v>62</v>
       </c>
       <c r="R21" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S21" s="39" t="s">
         <v>87</v>
@@ -3729,7 +3729,7 @@
         <v>62</v>
       </c>
       <c r="R22" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S22" s="39" t="s">
         <v>87</v>
@@ -3790,7 +3790,7 @@
         <v>62</v>
       </c>
       <c r="R23" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S23" s="39" t="s">
         <v>87</v>
@@ -3851,7 +3851,7 @@
         <v>62</v>
       </c>
       <c r="R24" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S24" s="39" t="s">
         <v>87</v>
@@ -3912,7 +3912,7 @@
         <v>62</v>
       </c>
       <c r="R25" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S25" s="39" t="s">
         <v>87</v>
@@ -8127,11 +8127,11 @@
   </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -8191,13 +8191,13 @@
   </sheetPr>
   <dimension ref="A1:G960"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
@@ -9341,11 +9341,11 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.17"/>

</xml_diff>

<commit_message>
Commit Anatomia Patologica - aggiornamento check list
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/MedicaRAP/3.3.0.0/accreditamento-checklist_V8.2.6.1.xlsx
+++ b/GATEWAY/A1#111MULTIMEDIAS/MultimediaSrl/MedicaRAP/3.3.0.0/accreditamento-checklist_V8.2.6.1.xlsx
@@ -1554,7 +1554,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.82"/>
@@ -1641,7 +1641,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.18"/>
@@ -2715,14 +2715,14 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="R33" activeCellId="0" sqref="R33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
@@ -4020,7 +4020,7 @@
         <v>62</v>
       </c>
       <c r="R27" s="33" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="S27" s="39" t="s">
         <v>87</v>
@@ -8131,7 +8131,7 @@
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -8197,7 +8197,7 @@
       <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.81"/>
@@ -9345,7 +9345,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.17"/>

</xml_diff>